<commit_message>
Intergrated Twilio API (#4)
Intergrated Twilio API and implemented SMS sending functionality.
</commit_message>
<xml_diff>
--- a/Forum_DB.xlsx
+++ b/Forum_DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Python\DueDate_Notification_vid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A1C23E-A603-4886-881F-7E2F201DD8E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628838A4-C16A-42DF-9B0A-F551092F4056}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,9 +76,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -104,9 +110,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,14 +433,15 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D2" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="11.5703125"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -461,9 +471,7 @@
       <c r="C2" s="1">
         <v>43926</v>
       </c>
-      <c r="D2">
-        <v>90000001</v>
-      </c>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -475,9 +483,7 @@
       <c r="C3" s="1">
         <v>43927</v>
       </c>
-      <c r="D3">
-        <v>90000002</v>
-      </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -489,9 +495,7 @@
       <c r="C4" s="1">
         <v>43928</v>
       </c>
-      <c r="D4">
-        <v>90000003</v>
-      </c>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -503,9 +507,7 @@
       <c r="C5" s="1">
         <v>43929</v>
       </c>
-      <c r="D5">
-        <v>90000004</v>
-      </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -517,9 +519,7 @@
       <c r="C6" s="1">
         <v>43895</v>
       </c>
-      <c r="D6">
-        <v>90000005</v>
-      </c>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -531,9 +531,7 @@
       <c r="C7" s="1">
         <v>43918</v>
       </c>
-      <c r="D7">
-        <v>90000006</v>
-      </c>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -545,9 +543,7 @@
       <c r="C8" s="1">
         <v>43926</v>
       </c>
-      <c r="D8">
-        <v>90000007</v>
-      </c>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -559,9 +555,7 @@
       <c r="C9" s="1">
         <v>43926</v>
       </c>
-      <c r="D9">
-        <v>90000008</v>
-      </c>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -573,9 +567,7 @@
       <c r="C10" s="1">
         <v>43926</v>
       </c>
-      <c r="D10">
-        <v>90000009</v>
-      </c>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -587,13 +579,12 @@
       <c r="C11" s="1">
         <v>43926</v>
       </c>
-      <c r="D11">
-        <v>90000010</v>
-      </c>
+      <c r="D11" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>